<commit_message>
successfully uploaded and resent flattened file =)
</commit_message>
<xml_diff>
--- a/uploads/FLAT_2016_06_DigitalPlayground.xlsx
+++ b/uploads/FLAT_2016_06_DigitalPlayground.xlsx
@@ -1095,7 +1095,7 @@
     <t>0630809|0630809</t>
   </si>
   <si>
-    <t>Eva Lovia, Kleio Valentien, Alyssa Divine</t>
+    <t>Alyssa Divine, Kleio Valentien, Eva Lovia</t>
   </si>
   <si>
     <t>xxx_raw_cuts_11</t>
@@ -1116,7 +1116,7 @@
     <t>0630810|0630810</t>
   </si>
   <si>
-    <t>Alexia Gold, Tysen Rich, Stevie Shae, Jessie Parker</t>
+    <t>Alexia Gold, Tysen Rich, Jessie Parker, Stevie Shae</t>
   </si>
   <si>
     <t>bad_girls_3</t>
@@ -1332,7 +1332,7 @@
     <t>media_sourced_from</t>
   </si>
   <si>
-    <t>02/18/2016 02:37:00</t>
+    <t>02/18/2016 03:04:35</t>
   </si>
 </sst>
 </file>
@@ -7028,7 +7028,7 @@
         <v>54</v>
       </c>
       <c r="C9" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -7081,7 +7081,7 @@
         <v>55</v>
       </c>
       <c r="C10" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -7134,7 +7134,7 @@
         <v>56</v>
       </c>
       <c r="C11" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -7187,7 +7187,7 @@
         <v>54</v>
       </c>
       <c r="C12" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -7234,7 +7234,7 @@
         <v>57</v>
       </c>
       <c r="C13" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -7287,7 +7287,7 @@
         <v>58</v>
       </c>
       <c r="C14" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -7340,7 +7340,7 @@
         <v>59</v>
       </c>
       <c r="C15" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -7393,7 +7393,7 @@
         <v>60</v>
       </c>
       <c r="C16" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -7446,7 +7446,7 @@
         <v>57</v>
       </c>
       <c r="C17" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>

</xml_diff>